<commit_message>
Change test input files to add commodity column
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/multiregion_macro_input.xlsx
+++ b/message_ix/tests/data/multiregion_macro_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\message_ix\message_ix\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unlu\Documents\GitHub\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476E6F3-03DE-4643-BFE3-09CF9C6645BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE6EE1D-C956-4955-B240-902084FDF7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1410" yWindow="390" windowWidth="21600" windowHeight="12360" tabRatio="992" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="8505" yWindow="2550" windowWidth="12435" windowHeight="8730" tabRatio="992" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="18">
   <si>
     <t>node</t>
   </si>
@@ -94,6 +94,9 @@
   </si>
   <si>
     <t>useful</t>
+  </si>
+  <si>
+    <t>commodity</t>
   </si>
 </sst>
 </file>
@@ -1029,7 +1032,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="L22" sqref="L22"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,15 +1178,17 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:D3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="G14" sqref="G14"/>
+      <selection activeCell="D4" sqref="D4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1025" width="11.5703125"/>
+    <col min="1" max="2" width="11.5703125"/>
+    <col min="3" max="3" width="11" bestFit="1" customWidth="1"/>
+    <col min="4" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.25">
@@ -1194,10 +1199,10 @@
         <v>1</v>
       </c>
       <c r="C1" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" t="s">
         <v>15</v>
-      </c>
-      <c r="D1" t="s">
-        <v>9</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.25">
@@ -1208,10 +1213,10 @@
         <v>5</v>
       </c>
       <c r="C2" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" t="s">
         <v>16</v>
-      </c>
-      <c r="D2">
-        <v>2020</v>
       </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.25">
@@ -1221,13 +1226,11 @@
       <c r="B3" t="s">
         <v>6</v>
       </c>
-      <c r="D3">
-        <v>2030</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="D4">
-        <v>2040</v>
+      <c r="C3" t="s">
+        <v>5</v>
+      </c>
+      <c r="D3" t="s">
+        <v>16</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read MACRO years directly from config of Excel
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/multiregion_macro_input.xlsx
+++ b/message_ix/tests/data/multiregion_macro_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="21929"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5C715E4D-6493-4102-AC37-95EC784746EB}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E476E6F3-03DE-4643-BFE3-09CF9C6645BD}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="12270" tabRatio="992" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1410" yWindow="390" windowWidth="21600" windowHeight="12360" tabRatio="992" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="17">
   <si>
     <t>node</t>
   </si>
@@ -1029,7 +1029,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="L22" sqref="L22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1175,10 +1175,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:D4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="G14" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1186,7 +1186,7 @@
     <col min="1" max="1025" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1196,8 +1196,11 @@
       <c r="C1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1207,13 +1210,24 @@
       <c r="C2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="D2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
       <c r="B3" t="s">
         <v>6</v>
+      </c>
+      <c r="D3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="D4">
+        <v>2040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Read data from Excel config flexibly for desirable years
</commit_message>
<xml_diff>
--- a/message_ix/tests/data/multiregion_macro_input.xlsx
+++ b/message_ix/tests/data/multiregion_macro_input.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24026"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23628"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\unlu\Documents\GitHub\message_ix\message_ix\tests\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\zakeri\Documents\Github\message_ix\message_ix\tests\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5EE6EE1D-C956-4955-B240-902084FDF7A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FF58AB80-9635-4009-B3D0-0578D1384A30}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="8505" yWindow="2550" windowWidth="12435" windowHeight="8730" tabRatio="992" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="840" yWindow="345" windowWidth="21600" windowHeight="12360" tabRatio="992" firstSheet="4" activeTab="12" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="price_ref" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="204" uniqueCount="18">
   <si>
     <t>node</t>
   </si>
@@ -571,7 +571,7 @@
   <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D3" sqref="D3:D9"/>
+      <selection activeCell="B3" sqref="B3:B5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1178,10 +1178,10 @@
 
 <file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0C00-000000000000}">
-  <dimension ref="A1:D3"/>
+  <dimension ref="A1:E4"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D4" sqref="D4"/>
+      <selection activeCell="E2" sqref="E2:E4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1191,7 +1191,7 @@
     <col min="4" max="1026" width="11.5703125"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1204,8 +1204,11 @@
       <c r="D1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E1" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>4</v>
       </c>
@@ -1218,8 +1221,11 @@
       <c r="D2" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+      <c r="E2">
+        <v>2020</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>7</v>
       </c>
@@ -1231,6 +1237,14 @@
       </c>
       <c r="D3" t="s">
         <v>16</v>
+      </c>
+      <c r="E3">
+        <v>2030</v>
+      </c>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="E4">
+        <v>2040</v>
       </c>
     </row>
   </sheetData>

</xml_diff>